<commit_message>
V17.4 poprawka z zerowaniem punktów
</commit_message>
<xml_diff>
--- a/ranking.xlsx
+++ b/ranking.xlsx
@@ -457,11 +457,11 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>testowańsko</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -471,7 +471,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -480,11 +480,11 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>j</t>
+          <t>l</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -494,7 +494,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -503,11 +503,11 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ty</t>
+          <t>j</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -526,11 +526,11 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>testowańsko</t>
+          <t>ty</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -549,7 +549,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -572,7 +572,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -618,11 +618,11 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11111</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -632,7 +632,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -645,7 +645,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>11111</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -655,11 +655,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -678,11 +678,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12">
@@ -691,7 +691,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -701,11 +701,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13">
@@ -714,7 +714,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -724,48 +724,48 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -783,7 +783,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>l</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -793,11 +793,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
@@ -806,7 +806,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -816,11 +816,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
@@ -829,7 +829,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>testyyyyyyy</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -839,11 +839,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
@@ -852,21 +852,21 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>testyyyyyyy</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20">
@@ -875,21 +875,21 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21">
@@ -898,21 +898,21 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22">
@@ -921,7 +921,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Karolcio</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -944,7 +944,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Karolcio</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -954,7 +954,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Wielkopolskie</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -967,28 +967,32 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="inlineStr"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -996,22 +1000,18 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1028,21 +1028,21 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1051,39 +1051,35 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>szymek</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>kkk</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1101,17 +1097,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>szymek</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1120,12 +1116,16 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B31" t="inlineStr"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>kkk</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1139,34 +1139,34 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1185,21 +1185,21 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1208,9 +1208,13 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr"/>
+        <v>36</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1218,7 +1222,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1227,13 +1231,9 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1250,11 +1250,11 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1273,21 +1273,21 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>uj</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1296,21 +1296,21 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>uj</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1319,11 +1319,11 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1333,20 +1333,20 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>'</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1356,7 +1356,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -1367,7 +1367,11 @@
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>'</t>
+        </is>
+      </c>
       <c r="C42" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1375,11 +1379,11 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43">
@@ -1389,16 +1393,16 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44">
@@ -1430,7 +1434,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1440,34 +1444,30 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>iu</t>
-        </is>
-      </c>
+      <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47">
@@ -1486,18 +1486,22 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>iu</t>
+        </is>
+      </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1509,7 +1513,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49">
@@ -1528,7 +1532,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -1539,11 +1543,7 @@
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
+      <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1551,11 +1551,11 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1574,11 +1574,11 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V17.5 kolejna porcja poprawek
</commit_message>
<xml_diff>
--- a/ranking.xlsx
+++ b/ranking.xlsx
@@ -457,11 +457,11 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>testowańsko</t>
+          <t>Gracz 3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,11 +480,11 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>Gracz 5</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -503,11 +503,11 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>j</t>
+          <t>Gracz test</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -526,11 +526,11 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ty</t>
+          <t>Gracz 1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -563,20 +563,20 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>'</t>
+          <t>Gracz 11</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -595,11 +595,11 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>testowańsko</t>
+          <t>Gracz a</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -618,11 +618,11 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>Gracz 8</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -632,20 +632,20 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11111</t>
+          <t>Gracz 26</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -655,7 +655,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -664,11 +664,11 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>Gracz test 2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -678,20 +678,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -701,20 +701,20 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -724,20 +724,20 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -747,48 +747,48 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -802,11 +802,11 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>l</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -816,20 +816,20 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -839,20 +839,20 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>testyyyyyyy</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -862,66 +862,66 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>testyyyyyyy</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -931,16 +931,16 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -990,7 +990,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1000,18 +1000,22 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B26" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1019,16 +1023,16 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1051,21 +1055,17 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1076,19 +1076,23 @@
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30">
@@ -1097,17 +1101,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>szymek</t>
+          <t>kkk</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1120,12 +1124,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>kkk</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1139,16 +1143,12 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1162,25 +1162,25 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>szymek</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Kujawsko-Pomorskie</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
         <v>35</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>hjk</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Extreme</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Lubelskie</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
-        <v>33</v>
       </c>
     </row>
     <row r="34">
@@ -1189,17 +1189,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1208,11 +1208,11 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1231,9 +1231,13 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B36" t="inlineStr"/>
+        <v>40</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
       <c r="C36" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1241,7 +1245,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -1250,11 +1254,11 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1264,7 +1268,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -1273,13 +1277,9 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -1296,21 +1296,21 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>uj</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -1319,21 +1319,21 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>uj</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1342,11 +1342,11 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>d</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1356,20 +1356,20 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>'</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1379,30 +1379,34 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr"/>
+        <v>33</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44">
@@ -1411,7 +1415,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1421,11 +1425,11 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45">
@@ -1434,7 +1438,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>'</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1444,11 +1448,11 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46">
@@ -1458,16 +1462,16 @@
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47">
@@ -1476,7 +1480,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1486,34 +1490,30 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>iu</t>
-        </is>
-      </c>
+      <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1532,18 +1532,22 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1551,11 +1555,11 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51">
@@ -1564,7 +1568,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>iu</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1574,11 +1578,11 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>